<commit_message>
user-manual and full-screen-svg 25x25/50x50 added
</commit_message>
<xml_diff>
--- a/Hardware/Snake_Array.xlsx
+++ b/Hardware/Snake_Array.xlsx
@@ -1,42 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ieu\HTML5\WordClock\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtyed\Documents\HTML5\WordClock\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24B93CD-4585-45CB-91F5-107CCA88AA3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2B17E9-E9A3-46DB-85FE-0214267D3F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{7E3663BD-6B5D-4282-8822-3089C3392D79}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7E3663BD-6B5D-4282-8822-3089C3392D79}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Snake_Array" sheetId="1" r:id="rId1"/>
+    <sheet name="Abmessungen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t>Zeile bestimmen: kürzen (x/11)</t>
   </si>
@@ -78,6 +68,27 @@
   </si>
   <si>
     <t>kürzen (x/11) = kürzen (y / 11)</t>
+  </si>
+  <si>
+    <t>Modell 25x25</t>
+  </si>
+  <si>
+    <t>Modell 50x50</t>
+  </si>
+  <si>
+    <t>SVG Original</t>
+  </si>
+  <si>
+    <t>25*25</t>
+  </si>
+  <si>
+    <t>rand verschieben</t>
+  </si>
+  <si>
+    <t>Breite</t>
+  </si>
+  <si>
+    <t>Höhe</t>
   </si>
 </sst>
 </file>
@@ -135,47 +146,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFB9B9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -213,221 +184,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9F9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9F9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9F9F"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8AEAE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8AEAE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -761,9 +517,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E0CD50-CE68-4D41-8ADF-D56E7A202DFA}">
   <dimension ref="B1:AJ19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -814,91 +568,91 @@
       <c r="L2" s="1">
         <v>10</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="1">
         <f>TRUNC(B2/11)</f>
         <v>0</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="1">
         <f t="shared" ref="O2:X2" si="0">TRUNC(C2/11)</f>
         <v>0</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="1">
         <f>MOD(B2,11)</f>
         <v>0</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="1">
         <f t="shared" ref="AA2:AJ2" si="1">MOD(C2,11)</f>
         <v>1</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="1">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="1">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="1">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="1">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="1">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="1">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="1">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
@@ -937,91 +691,91 @@
       <c r="L3" s="1">
         <v>11</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="1">
         <f t="shared" ref="N3:N12" si="2">TRUNC(B3/11)</f>
         <v>1</v>
       </c>
-      <c r="O3">
+      <c r="O3" s="1">
         <f t="shared" ref="O3:O12" si="3">TRUNC(C3/11)</f>
         <v>1</v>
       </c>
-      <c r="P3">
+      <c r="P3" s="1">
         <f t="shared" ref="P3:P12" si="4">TRUNC(D3/11)</f>
         <v>1</v>
       </c>
-      <c r="Q3">
+      <c r="Q3" s="1">
         <f t="shared" ref="Q3:Q12" si="5">TRUNC(E3/11)</f>
         <v>1</v>
       </c>
-      <c r="R3">
+      <c r="R3" s="1">
         <f t="shared" ref="R3:R12" si="6">TRUNC(F3/11)</f>
         <v>1</v>
       </c>
-      <c r="S3">
+      <c r="S3" s="1">
         <f t="shared" ref="S3:S12" si="7">TRUNC(G3/11)</f>
         <v>1</v>
       </c>
-      <c r="T3">
+      <c r="T3" s="1">
         <f t="shared" ref="T3:T12" si="8">TRUNC(H3/11)</f>
         <v>1</v>
       </c>
-      <c r="U3">
+      <c r="U3" s="1">
         <f t="shared" ref="U3:U12" si="9">TRUNC(I3/11)</f>
         <v>1</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="1">
         <f t="shared" ref="V3:V12" si="10">TRUNC(J3/11)</f>
         <v>1</v>
       </c>
-      <c r="W3">
+      <c r="W3" s="1">
         <f t="shared" ref="W3:W12" si="11">TRUNC(K3/11)</f>
         <v>1</v>
       </c>
-      <c r="X3">
+      <c r="X3" s="1">
         <f t="shared" ref="X3:X12" si="12">TRUNC(L3/11)</f>
         <v>1</v>
       </c>
-      <c r="Z3">
+      <c r="Z3" s="1">
         <f t="shared" ref="Z3:Z12" si="13">MOD(B3,11)</f>
         <v>10</v>
       </c>
-      <c r="AA3">
+      <c r="AA3" s="1">
         <f t="shared" ref="AA3:AA12" si="14">MOD(C3,11)</f>
         <v>9</v>
       </c>
-      <c r="AB3">
+      <c r="AB3" s="1">
         <f t="shared" ref="AB3:AB12" si="15">MOD(D3,11)</f>
         <v>8</v>
       </c>
-      <c r="AC3">
+      <c r="AC3" s="1">
         <f t="shared" ref="AC3:AC12" si="16">MOD(E3,11)</f>
         <v>7</v>
       </c>
-      <c r="AD3">
+      <c r="AD3" s="1">
         <f t="shared" ref="AD3:AD12" si="17">MOD(F3,11)</f>
         <v>6</v>
       </c>
-      <c r="AE3">
+      <c r="AE3" s="1">
         <f t="shared" ref="AE3:AE12" si="18">MOD(G3,11)</f>
         <v>5</v>
       </c>
-      <c r="AF3">
+      <c r="AF3" s="1">
         <f t="shared" ref="AF3:AF12" si="19">MOD(H3,11)</f>
         <v>4</v>
       </c>
-      <c r="AG3">
+      <c r="AG3" s="1">
         <f t="shared" ref="AG3:AG12" si="20">MOD(I3,11)</f>
         <v>3</v>
       </c>
-      <c r="AH3">
+      <c r="AH3" s="1">
         <f t="shared" ref="AH3:AH12" si="21">MOD(J3,11)</f>
         <v>2</v>
       </c>
-      <c r="AI3">
+      <c r="AI3" s="1">
         <f t="shared" ref="AI3:AI12" si="22">MOD(K3,11)</f>
         <v>1</v>
       </c>
-      <c r="AJ3">
+      <c r="AJ3" s="1">
         <f t="shared" ref="AJ3:AJ12" si="23">MOD(L3,11)</f>
         <v>0</v>
       </c>
@@ -1060,91 +814,91 @@
       <c r="L4" s="1">
         <v>32</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="1">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="1">
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="1">
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="1">
         <f t="shared" si="5"/>
         <v>2</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="1">
         <f t="shared" si="6"/>
         <v>2</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="1">
         <f t="shared" si="7"/>
         <v>2</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="1">
         <f t="shared" si="8"/>
         <v>2</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="1">
         <f t="shared" si="9"/>
         <v>2</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="1">
         <f t="shared" si="10"/>
         <v>2</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="1">
         <f t="shared" si="11"/>
         <v>2</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="1">
         <f t="shared" si="12"/>
         <v>2</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="1">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="1">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="1">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="1">
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="1">
         <f t="shared" si="19"/>
         <v>6</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="1">
         <f t="shared" si="20"/>
         <v>7</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="1">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="1">
         <f t="shared" si="22"/>
         <v>9</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="1">
         <f t="shared" si="23"/>
         <v>10</v>
       </c>
@@ -1183,91 +937,91 @@
       <c r="L5" s="1">
         <v>33</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="1">
         <f t="shared" si="2"/>
         <v>3</v>
       </c>
-      <c r="O5">
+      <c r="O5" s="1">
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="1">
         <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="Q5">
+      <c r="Q5" s="1">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="R5">
+      <c r="R5" s="1">
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="S5">
+      <c r="S5" s="1">
         <f t="shared" si="7"/>
         <v>3</v>
       </c>
-      <c r="T5">
+      <c r="T5" s="1">
         <f t="shared" si="8"/>
         <v>3</v>
       </c>
-      <c r="U5">
+      <c r="U5" s="1">
         <f t="shared" si="9"/>
         <v>3</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="1">
         <f t="shared" si="10"/>
         <v>3</v>
       </c>
-      <c r="W5">
+      <c r="W5" s="1">
         <f t="shared" si="11"/>
         <v>3</v>
       </c>
-      <c r="X5">
+      <c r="X5" s="1">
         <f t="shared" si="12"/>
         <v>3</v>
       </c>
-      <c r="Z5">
+      <c r="Z5" s="1">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="AA5">
+      <c r="AA5" s="1">
         <f t="shared" si="14"/>
         <v>9</v>
       </c>
-      <c r="AB5">
+      <c r="AB5" s="1">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="AC5">
+      <c r="AC5" s="1">
         <f t="shared" si="16"/>
         <v>7</v>
       </c>
-      <c r="AD5">
+      <c r="AD5" s="1">
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
-      <c r="AE5">
+      <c r="AE5" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF5">
+      <c r="AF5" s="1">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="AG5">
+      <c r="AG5" s="1">
         <f t="shared" si="20"/>
         <v>3</v>
       </c>
-      <c r="AH5">
+      <c r="AH5" s="1">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="AI5">
+      <c r="AI5" s="1">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="AJ5">
+      <c r="AJ5" s="1">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -1306,91 +1060,91 @@
       <c r="L6" s="1">
         <v>54</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="1">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="O6">
+      <c r="O6" s="1">
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P6">
+      <c r="P6" s="1">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="1">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="R6">
+      <c r="R6" s="1">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="1">
         <f t="shared" si="7"/>
         <v>4</v>
       </c>
-      <c r="T6">
+      <c r="T6" s="1">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
-      <c r="U6">
+      <c r="U6" s="1">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="1">
         <f t="shared" si="10"/>
         <v>4</v>
       </c>
-      <c r="W6">
+      <c r="W6" s="1">
         <f t="shared" si="11"/>
         <v>4</v>
       </c>
-      <c r="X6">
+      <c r="X6" s="1">
         <f t="shared" si="12"/>
         <v>4</v>
       </c>
-      <c r="Z6">
+      <c r="Z6" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AA6">
+      <c r="AA6" s="1">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="AB6">
+      <c r="AB6" s="1">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="AC6">
+      <c r="AC6" s="1">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="AD6">
+      <c r="AD6" s="1">
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="AE6">
+      <c r="AE6" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF6">
+      <c r="AF6" s="1">
         <f t="shared" si="19"/>
         <v>6</v>
       </c>
-      <c r="AG6">
+      <c r="AG6" s="1">
         <f t="shared" si="20"/>
         <v>7</v>
       </c>
-      <c r="AH6">
+      <c r="AH6" s="1">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="AI6">
+      <c r="AI6" s="1">
         <f t="shared" si="22"/>
         <v>9</v>
       </c>
-      <c r="AJ6">
+      <c r="AJ6" s="1">
         <f t="shared" si="23"/>
         <v>10</v>
       </c>
@@ -1429,91 +1183,91 @@
       <c r="L7" s="1">
         <v>55</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="1">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="O7">
+      <c r="O7" s="1">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="P7">
+      <c r="P7" s="1">
         <f t="shared" si="4"/>
         <v>5</v>
       </c>
-      <c r="Q7">
+      <c r="Q7" s="1">
         <f t="shared" si="5"/>
         <v>5</v>
       </c>
-      <c r="R7">
+      <c r="R7" s="1">
         <f t="shared" si="6"/>
         <v>5</v>
       </c>
-      <c r="S7">
+      <c r="S7" s="1">
         <f t="shared" si="7"/>
         <v>5</v>
       </c>
-      <c r="T7">
+      <c r="T7" s="1">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
-      <c r="U7">
+      <c r="U7" s="1">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="1">
         <f t="shared" si="10"/>
         <v>5</v>
       </c>
-      <c r="W7">
+      <c r="W7" s="1">
         <f t="shared" si="11"/>
         <v>5</v>
       </c>
-      <c r="X7">
+      <c r="X7" s="1">
         <f t="shared" si="12"/>
         <v>5</v>
       </c>
-      <c r="Z7">
+      <c r="Z7" s="1">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="AA7">
+      <c r="AA7" s="1">
         <f t="shared" si="14"/>
         <v>9</v>
       </c>
-      <c r="AB7">
+      <c r="AB7" s="1">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="AC7">
+      <c r="AC7" s="1">
         <f t="shared" si="16"/>
         <v>7</v>
       </c>
-      <c r="AD7">
+      <c r="AD7" s="1">
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
-      <c r="AE7">
+      <c r="AE7" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF7">
+      <c r="AF7" s="1">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="AG7">
+      <c r="AG7" s="1">
         <f t="shared" si="20"/>
         <v>3</v>
       </c>
-      <c r="AH7">
+      <c r="AH7" s="1">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="AI7">
+      <c r="AI7" s="1">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="AJ7">
+      <c r="AJ7" s="1">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -1552,91 +1306,91 @@
       <c r="L8" s="1">
         <v>76</v>
       </c>
-      <c r="N8">
+      <c r="N8" s="1">
         <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="O8">
+      <c r="O8" s="1">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="P8">
+      <c r="P8" s="1">
         <f t="shared" si="4"/>
         <v>6</v>
       </c>
-      <c r="Q8">
+      <c r="Q8" s="1">
         <f t="shared" si="5"/>
         <v>6</v>
       </c>
-      <c r="R8">
+      <c r="R8" s="1">
         <f t="shared" si="6"/>
         <v>6</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="1">
         <f t="shared" si="7"/>
         <v>6</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="1">
         <f t="shared" si="8"/>
         <v>6</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="1">
         <f t="shared" si="9"/>
         <v>6</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="1">
         <f t="shared" si="10"/>
         <v>6</v>
       </c>
-      <c r="W8">
+      <c r="W8" s="1">
         <f t="shared" si="11"/>
         <v>6</v>
       </c>
-      <c r="X8">
+      <c r="X8" s="1">
         <f t="shared" si="12"/>
         <v>6</v>
       </c>
-      <c r="Z8">
+      <c r="Z8" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AA8">
+      <c r="AA8" s="1">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="AB8">
+      <c r="AB8" s="1">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="AC8">
+      <c r="AC8" s="1">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="AD8">
+      <c r="AD8" s="1">
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="AE8">
+      <c r="AE8" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF8">
+      <c r="AF8" s="1">
         <f t="shared" si="19"/>
         <v>6</v>
       </c>
-      <c r="AG8">
+      <c r="AG8" s="1">
         <f t="shared" si="20"/>
         <v>7</v>
       </c>
-      <c r="AH8">
+      <c r="AH8" s="1">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="AI8">
+      <c r="AI8" s="1">
         <f t="shared" si="22"/>
         <v>9</v>
       </c>
-      <c r="AJ8">
+      <c r="AJ8" s="1">
         <f t="shared" si="23"/>
         <v>10</v>
       </c>
@@ -1675,91 +1429,91 @@
       <c r="L9" s="1">
         <v>77</v>
       </c>
-      <c r="N9">
+      <c r="N9" s="1">
         <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="O9">
+      <c r="O9" s="1">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="P9">
+      <c r="P9" s="1">
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-      <c r="Q9">
+      <c r="Q9" s="1">
         <f t="shared" si="5"/>
         <v>7</v>
       </c>
-      <c r="R9">
+      <c r="R9" s="1">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="1">
         <f t="shared" si="7"/>
         <v>7</v>
       </c>
-      <c r="T9">
+      <c r="T9" s="1">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
-      <c r="U9">
+      <c r="U9" s="1">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="1">
         <f t="shared" si="10"/>
         <v>7</v>
       </c>
-      <c r="W9">
+      <c r="W9" s="1">
         <f t="shared" si="11"/>
         <v>7</v>
       </c>
-      <c r="X9">
+      <c r="X9" s="1">
         <f t="shared" si="12"/>
         <v>7</v>
       </c>
-      <c r="Z9">
+      <c r="Z9" s="1">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="AA9">
+      <c r="AA9" s="1">
         <f t="shared" si="14"/>
         <v>9</v>
       </c>
-      <c r="AB9">
+      <c r="AB9" s="1">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="AC9">
+      <c r="AC9" s="1">
         <f t="shared" si="16"/>
         <v>7</v>
       </c>
-      <c r="AD9">
+      <c r="AD9" s="1">
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
-      <c r="AE9">
+      <c r="AE9" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF9">
+      <c r="AF9" s="1">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="AG9">
+      <c r="AG9" s="1">
         <f t="shared" si="20"/>
         <v>3</v>
       </c>
-      <c r="AH9">
+      <c r="AH9" s="1">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="AI9">
+      <c r="AI9" s="1">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="AJ9">
+      <c r="AJ9" s="1">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -1798,91 +1552,91 @@
       <c r="L10" s="1">
         <v>98</v>
       </c>
-      <c r="N10">
+      <c r="N10" s="1">
         <f t="shared" si="2"/>
         <v>8</v>
       </c>
-      <c r="O10">
+      <c r="O10" s="1">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="P10">
+      <c r="P10" s="1">
         <f t="shared" si="4"/>
         <v>8</v>
       </c>
-      <c r="Q10">
+      <c r="Q10" s="1">
         <f t="shared" si="5"/>
         <v>8</v>
       </c>
-      <c r="R10">
+      <c r="R10" s="1">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="1">
         <f t="shared" si="7"/>
         <v>8</v>
       </c>
-      <c r="T10">
+      <c r="T10" s="1">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
-      <c r="U10">
+      <c r="U10" s="1">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="1">
         <f t="shared" si="10"/>
         <v>8</v>
       </c>
-      <c r="W10">
+      <c r="W10" s="1">
         <f t="shared" si="11"/>
         <v>8</v>
       </c>
-      <c r="X10">
+      <c r="X10" s="1">
         <f t="shared" si="12"/>
         <v>8</v>
       </c>
-      <c r="Z10">
+      <c r="Z10" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AA10">
+      <c r="AA10" s="1">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="AB10">
+      <c r="AB10" s="1">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="AC10">
+      <c r="AC10" s="1">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="AD10">
+      <c r="AD10" s="1">
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="AE10">
+      <c r="AE10" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF10">
+      <c r="AF10" s="1">
         <f t="shared" si="19"/>
         <v>6</v>
       </c>
-      <c r="AG10">
+      <c r="AG10" s="1">
         <f t="shared" si="20"/>
         <v>7</v>
       </c>
-      <c r="AH10">
+      <c r="AH10" s="1">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="AI10">
+      <c r="AI10" s="1">
         <f t="shared" si="22"/>
         <v>9</v>
       </c>
-      <c r="AJ10">
+      <c r="AJ10" s="1">
         <f t="shared" si="23"/>
         <v>10</v>
       </c>
@@ -1921,91 +1675,91 @@
       <c r="L11" s="1">
         <v>99</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="1">
         <f t="shared" si="2"/>
         <v>9</v>
       </c>
-      <c r="O11">
+      <c r="O11" s="1">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="P11">
+      <c r="P11" s="1">
         <f t="shared" si="4"/>
         <v>9</v>
       </c>
-      <c r="Q11">
+      <c r="Q11" s="1">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="R11">
+      <c r="R11" s="1">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="1">
         <f t="shared" si="7"/>
         <v>9</v>
       </c>
-      <c r="T11">
+      <c r="T11" s="1">
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
-      <c r="U11">
+      <c r="U11" s="1">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="1">
         <f t="shared" si="10"/>
         <v>9</v>
       </c>
-      <c r="W11">
+      <c r="W11" s="1">
         <f t="shared" si="11"/>
         <v>9</v>
       </c>
-      <c r="X11">
+      <c r="X11" s="1">
         <f t="shared" si="12"/>
         <v>9</v>
       </c>
-      <c r="Z11">
+      <c r="Z11" s="1">
         <f t="shared" si="13"/>
         <v>10</v>
       </c>
-      <c r="AA11">
+      <c r="AA11" s="1">
         <f t="shared" si="14"/>
         <v>9</v>
       </c>
-      <c r="AB11">
+      <c r="AB11" s="1">
         <f t="shared" si="15"/>
         <v>8</v>
       </c>
-      <c r="AC11">
+      <c r="AC11" s="1">
         <f t="shared" si="16"/>
         <v>7</v>
       </c>
-      <c r="AD11">
+      <c r="AD11" s="1">
         <f t="shared" si="17"/>
         <v>6</v>
       </c>
-      <c r="AE11">
+      <c r="AE11" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF11">
+      <c r="AF11" s="1">
         <f t="shared" si="19"/>
         <v>4</v>
       </c>
-      <c r="AG11">
+      <c r="AG11" s="1">
         <f t="shared" si="20"/>
         <v>3</v>
       </c>
-      <c r="AH11">
+      <c r="AH11" s="1">
         <f t="shared" si="21"/>
         <v>2</v>
       </c>
-      <c r="AI11">
+      <c r="AI11" s="1">
         <f t="shared" si="22"/>
         <v>1</v>
       </c>
-      <c r="AJ11">
+      <c r="AJ11" s="1">
         <f t="shared" si="23"/>
         <v>0</v>
       </c>
@@ -2044,91 +1798,91 @@
       <c r="L12" s="1">
         <v>120</v>
       </c>
-      <c r="N12">
+      <c r="N12" s="1">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
-      <c r="O12">
+      <c r="O12" s="1">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="P12">
+      <c r="P12" s="1">
         <f t="shared" si="4"/>
         <v>10</v>
       </c>
-      <c r="Q12">
+      <c r="Q12" s="1">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="R12">
+      <c r="R12" s="1">
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="S12">
+      <c r="S12" s="1">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="T12">
+      <c r="T12" s="1">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
-      <c r="U12">
+      <c r="U12" s="1">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="1">
         <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="W12">
+      <c r="W12" s="1">
         <f t="shared" si="11"/>
         <v>10</v>
       </c>
-      <c r="X12">
+      <c r="X12" s="1">
         <f t="shared" si="12"/>
         <v>10</v>
       </c>
-      <c r="Z12">
+      <c r="Z12" s="1">
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-      <c r="AA12">
+      <c r="AA12" s="1">
         <f t="shared" si="14"/>
         <v>1</v>
       </c>
-      <c r="AB12">
+      <c r="AB12" s="1">
         <f t="shared" si="15"/>
         <v>2</v>
       </c>
-      <c r="AC12">
+      <c r="AC12" s="1">
         <f t="shared" si="16"/>
         <v>3</v>
       </c>
-      <c r="AD12">
+      <c r="AD12" s="1">
         <f t="shared" si="17"/>
         <v>4</v>
       </c>
-      <c r="AE12">
+      <c r="AE12" s="1">
         <f t="shared" si="18"/>
         <v>5</v>
       </c>
-      <c r="AF12">
+      <c r="AF12" s="1">
         <f t="shared" si="19"/>
         <v>6</v>
       </c>
-      <c r="AG12">
+      <c r="AG12" s="1">
         <f t="shared" si="20"/>
         <v>7</v>
       </c>
-      <c r="AH12">
+      <c r="AH12" s="1">
         <f t="shared" si="21"/>
         <v>8</v>
       </c>
-      <c r="AI12">
+      <c r="AI12" s="1">
         <f t="shared" si="22"/>
         <v>9</v>
       </c>
-      <c r="AJ12">
+      <c r="AJ12" s="1">
         <f t="shared" si="23"/>
         <v>10</v>
       </c>
@@ -2203,27 +1957,27 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:L12">
-    <cfRule type="cellIs" dxfId="8" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>$D$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>120</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula xml:space="preserve"> TRUNC($D$18/11)&lt;&gt;TRUNC($D$15/11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="4" priority="2">
+    <cfRule type="expression" dxfId="0" priority="2">
       <formula xml:space="preserve"> TRUNC($D$19/11)&lt;&gt;TRUNC($D$15/11)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2232,6 +1986,105 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C22D3B1-E60D-498D-9AAC-32F93F91DBF6}">
+  <dimension ref="A1:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>183.46</v>
+      </c>
+      <c r="B4">
+        <v>250</v>
+      </c>
+      <c r="C4">
+        <f>(B4-A4)/2</f>
+        <v>33.269999999999996</v>
+      </c>
+      <c r="F4">
+        <f>A4*2</f>
+        <v>366.92</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:H4" si="0">B4*2</f>
+        <v>500</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>66.539999999999992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>176.19</v>
+      </c>
+      <c r="B6">
+        <v>250</v>
+      </c>
+      <c r="C6">
+        <f>(B6-A6)/2</f>
+        <v>36.905000000000001</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ref="F6:H6" si="1">A6*2</f>
+        <v>352.38</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>73.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{36624f80-466a-4324-91bb-078ba1487887}" enabled="1" method="Privileged" siteId="{af7227b1-ac3a-4487-9e9f-ba462bb409d4}" contentBits="0" removed="0"/>

</xml_diff>

<commit_message>
Feature: Ghosthour initial release
</commit_message>
<xml_diff>
--- a/Hardware/Snake_Array.xlsx
+++ b/Hardware/Snake_Array.xlsx
@@ -1,25 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtyed\Documents\HTML5\WordClock\Hardware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ieu\HTML5\WordClock\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2B17E9-E9A3-46DB-85FE-0214267D3F9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB1A9FEF-7A8C-4354-8575-14567A5C366C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{7E3663BD-6B5D-4282-8822-3089C3392D79}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{7E3663BD-6B5D-4282-8822-3089C3392D79}"/>
   </bookViews>
   <sheets>
     <sheet name="Snake_Array" sheetId="1" r:id="rId1"/>
     <sheet name="Abmessungen" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -104,12 +115,30 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -139,14 +168,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FFC00000"/>
@@ -219,9 +261,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -259,7 +301,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -365,7 +407,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -507,7 +549,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -515,7 +557,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18E0CD50-CE68-4D41-8ADF-D56E7A202DFA}">
-  <dimension ref="B1:AJ19"/>
+  <dimension ref="B1:AJ39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1955,30 +1997,420 @@
         <v>13</v>
       </c>
     </row>
+    <row r="29" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3">
+        <v>0</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
+      </c>
+      <c r="D29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3">
+        <v>3</v>
+      </c>
+      <c r="F29" s="3">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
+      <c r="H29" s="2">
+        <v>6</v>
+      </c>
+      <c r="I29" s="2">
+        <v>7</v>
+      </c>
+      <c r="J29" s="3">
+        <v>8</v>
+      </c>
+      <c r="K29" s="3">
+        <v>9</v>
+      </c>
+      <c r="L29" s="3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="3">
+        <v>21</v>
+      </c>
+      <c r="C30" s="3">
+        <v>20</v>
+      </c>
+      <c r="D30" s="3">
+        <v>19</v>
+      </c>
+      <c r="E30" s="3">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2">
+        <v>17</v>
+      </c>
+      <c r="G30" s="2">
+        <v>16</v>
+      </c>
+      <c r="H30" s="2">
+        <v>15</v>
+      </c>
+      <c r="I30" s="3">
+        <v>14</v>
+      </c>
+      <c r="J30" s="3">
+        <v>13</v>
+      </c>
+      <c r="K30" s="3">
+        <v>12</v>
+      </c>
+      <c r="L30" s="3">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="3">
+        <v>22</v>
+      </c>
+      <c r="C31" s="3">
+        <v>23</v>
+      </c>
+      <c r="D31" s="3">
+        <v>24</v>
+      </c>
+      <c r="E31" s="2">
+        <v>25</v>
+      </c>
+      <c r="F31" s="2">
+        <v>26</v>
+      </c>
+      <c r="G31" s="2">
+        <v>27</v>
+      </c>
+      <c r="H31" s="2">
+        <v>28</v>
+      </c>
+      <c r="I31" s="2">
+        <v>29</v>
+      </c>
+      <c r="J31" s="3">
+        <v>30</v>
+      </c>
+      <c r="K31" s="3">
+        <v>31</v>
+      </c>
+      <c r="L31" s="3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="3">
+        <v>43</v>
+      </c>
+      <c r="C32" s="3">
+        <v>42</v>
+      </c>
+      <c r="D32" s="3">
+        <v>41</v>
+      </c>
+      <c r="E32" s="2">
+        <v>40</v>
+      </c>
+      <c r="F32" s="4">
+        <v>39</v>
+      </c>
+      <c r="G32" s="2">
+        <v>38</v>
+      </c>
+      <c r="H32" s="4">
+        <v>37</v>
+      </c>
+      <c r="I32" s="2">
+        <v>36</v>
+      </c>
+      <c r="J32" s="3">
+        <v>35</v>
+      </c>
+      <c r="K32" s="3">
+        <v>34</v>
+      </c>
+      <c r="L32" s="3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="2">
+        <v>44</v>
+      </c>
+      <c r="C33" s="3">
+        <v>45</v>
+      </c>
+      <c r="D33" s="3">
+        <v>46</v>
+      </c>
+      <c r="E33" s="2">
+        <v>47</v>
+      </c>
+      <c r="F33" s="4">
+        <v>48</v>
+      </c>
+      <c r="G33" s="2">
+        <v>49</v>
+      </c>
+      <c r="H33" s="4">
+        <v>50</v>
+      </c>
+      <c r="I33" s="2">
+        <v>51</v>
+      </c>
+      <c r="J33" s="3">
+        <v>52</v>
+      </c>
+      <c r="K33" s="2">
+        <v>53</v>
+      </c>
+      <c r="L33" s="2">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="2">
+        <v>65</v>
+      </c>
+      <c r="C34" s="2">
+        <v>64</v>
+      </c>
+      <c r="D34" s="2">
+        <v>63</v>
+      </c>
+      <c r="E34" s="2">
+        <v>62</v>
+      </c>
+      <c r="F34" s="2">
+        <v>61</v>
+      </c>
+      <c r="G34" s="3">
+        <v>60</v>
+      </c>
+      <c r="H34" s="2">
+        <v>59</v>
+      </c>
+      <c r="I34" s="2">
+        <v>58</v>
+      </c>
+      <c r="J34" s="2">
+        <v>57</v>
+      </c>
+      <c r="K34" s="2">
+        <v>56</v>
+      </c>
+      <c r="L34" s="2">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="3">
+        <v>66</v>
+      </c>
+      <c r="C35" s="2">
+        <v>67</v>
+      </c>
+      <c r="D35" s="2">
+        <v>68</v>
+      </c>
+      <c r="E35" s="2">
+        <v>69</v>
+      </c>
+      <c r="F35" s="2">
+        <v>70</v>
+      </c>
+      <c r="G35" s="3">
+        <v>71</v>
+      </c>
+      <c r="H35" s="2">
+        <v>72</v>
+      </c>
+      <c r="I35" s="2">
+        <v>73</v>
+      </c>
+      <c r="J35" s="2">
+        <v>74</v>
+      </c>
+      <c r="K35" s="2">
+        <v>75</v>
+      </c>
+      <c r="L35" s="3">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="3">
+        <v>87</v>
+      </c>
+      <c r="C36" s="3">
+        <v>86</v>
+      </c>
+      <c r="D36" s="2">
+        <v>85</v>
+      </c>
+      <c r="E36" s="2">
+        <v>84</v>
+      </c>
+      <c r="F36" s="2">
+        <v>83</v>
+      </c>
+      <c r="G36" s="2">
+        <v>82</v>
+      </c>
+      <c r="H36" s="2">
+        <v>81</v>
+      </c>
+      <c r="I36" s="2">
+        <v>80</v>
+      </c>
+      <c r="J36" s="2">
+        <v>79</v>
+      </c>
+      <c r="K36" s="3">
+        <v>78</v>
+      </c>
+      <c r="L36" s="3">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="3">
+        <v>88</v>
+      </c>
+      <c r="C37" s="3">
+        <v>89</v>
+      </c>
+      <c r="D37" s="3">
+        <v>90</v>
+      </c>
+      <c r="E37" s="2">
+        <v>91</v>
+      </c>
+      <c r="F37" s="2">
+        <v>92</v>
+      </c>
+      <c r="G37" s="2">
+        <v>93</v>
+      </c>
+      <c r="H37" s="2">
+        <v>94</v>
+      </c>
+      <c r="I37" s="2">
+        <v>95</v>
+      </c>
+      <c r="J37" s="3">
+        <v>96</v>
+      </c>
+      <c r="K37" s="3">
+        <v>97</v>
+      </c>
+      <c r="L37" s="3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="38" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="3">
+        <v>109</v>
+      </c>
+      <c r="C38" s="3">
+        <v>108</v>
+      </c>
+      <c r="D38" s="3">
+        <v>107</v>
+      </c>
+      <c r="E38" s="3">
+        <v>106</v>
+      </c>
+      <c r="F38" s="2">
+        <v>105</v>
+      </c>
+      <c r="G38" s="2">
+        <v>104</v>
+      </c>
+      <c r="H38" s="2">
+        <v>103</v>
+      </c>
+      <c r="I38" s="2">
+        <v>102</v>
+      </c>
+      <c r="J38" s="3">
+        <v>101</v>
+      </c>
+      <c r="K38" s="3">
+        <v>100</v>
+      </c>
+      <c r="L38" s="3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="3">
+        <v>110</v>
+      </c>
+      <c r="C39" s="3">
+        <v>111</v>
+      </c>
+      <c r="D39" s="3">
+        <v>112</v>
+      </c>
+      <c r="E39" s="3">
+        <v>113</v>
+      </c>
+      <c r="F39" s="3">
+        <v>114</v>
+      </c>
+      <c r="G39" s="3">
+        <v>115</v>
+      </c>
+      <c r="H39" s="2">
+        <v>116</v>
+      </c>
+      <c r="I39" s="2">
+        <v>117</v>
+      </c>
+      <c r="J39" s="2">
+        <v>118</v>
+      </c>
+      <c r="K39" s="3">
+        <v>119</v>
+      </c>
+      <c r="L39" s="3">
+        <v>120</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="B2:L12">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="equal">
       <formula>$D$15</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D16">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D17">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>120</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D18">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="2" priority="2">
       <formula xml:space="preserve"> TRUNC($D$18/11)&lt;&gt;TRUNC($D$15/11)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D19">
-    <cfRule type="expression" dxfId="0" priority="2">
+    <cfRule type="expression" dxfId="1" priority="3">
       <formula xml:space="preserve"> TRUNC($D$19/11)&lt;&gt;TRUNC($D$15/11)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:L39">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>$D$15</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
bugfix too many words
</commit_message>
<xml_diff>
--- a/Hardware/Snake_Array.xlsx
+++ b/Hardware/Snake_Array.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtyed\Documents\HTML5\WordClock\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF3AB14C-81E7-4281-8582-43BEA2A3CF47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B38547BA-11B2-48D7-A598-D52FD8CE8EFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="2" xr2:uid="{7E3663BD-6B5D-4282-8822-3089C3392D79}"/>
   </bookViews>
@@ -4234,6 +4234,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC8D6C3-2929-41CA-9874-7F411D5503A8}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:E537"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -6408,7 +6409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="208" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="208" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D208" t="s">
         <v>431</v>
       </c>
@@ -6795,7 +6796,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="251" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="251" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D251" t="s">
         <v>332</v>
       </c>
@@ -6804,7 +6805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="252" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D252" t="s">
         <v>235</v>
       </c>
@@ -6813,7 +6814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="253" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D253" t="s">
         <v>134</v>
       </c>
@@ -6822,7 +6823,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="254" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D254" t="s">
         <v>475</v>
       </c>
@@ -6831,7 +6832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="255" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D255" t="s">
         <v>335</v>
       </c>
@@ -6840,7 +6841,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="256" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D256" t="s">
         <v>241</v>
       </c>
@@ -6849,7 +6850,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="257" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D257" t="s">
         <v>362</v>
       </c>
@@ -6858,7 +6859,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="258" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D258" t="s">
         <v>481</v>
       </c>
@@ -6867,7 +6868,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="259" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D259" t="s">
         <v>480</v>
       </c>
@@ -8048,7 +8049,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="384" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="384" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D384" t="s">
         <v>399</v>
       </c>
@@ -8193,7 +8194,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="397" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="397" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D397" t="s">
         <v>451</v>
       </c>
@@ -8652,7 +8653,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="448" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="448" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D448" t="s">
         <v>214</v>
       </c>
@@ -8824,7 +8825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="464" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="464" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D464" t="s">
         <v>269</v>
       </c>
@@ -9040,7 +9041,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="488" spans="4:5" x14ac:dyDescent="0.45">
+    <row r="488" spans="4:5" hidden="1" x14ac:dyDescent="0.45">
       <c r="D488" t="s">
         <v>376</v>
       </c>
@@ -9516,7 +9517,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D4:E537" xr:uid="{8EC8D6C3-2929-41CA-9874-7F411D5503A8}"/>
+  <autoFilter ref="D4:E537" xr:uid="{8EC8D6C3-2929-41CA-9874-7F411D5503A8}">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="WAHR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D5:E1102">
     <sortCondition ref="D63:D1102"/>
   </sortState>

</xml_diff>